<commit_message>
Mapas de Chile y Colombia actualizados
</commit_message>
<xml_diff>
--- a/Map/Pobreza_2020Colombia.xlsx
+++ b/Map/Pobreza_2020Colombia.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanwen/Dropbox/youtube/3. Mapas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanwen/Dropbox/1. youtube/Season1/Map/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9897B3DC-085D-8741-854D-B92A5993AE34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{483903E8-0795-D841-82AE-A4566F6C3258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3760" yWindow="1500" windowWidth="25040" windowHeight="14500" xr2:uid="{B5A9D9C6-0E32-834A-AB46-51FBAA8D7782}"/>
+    <workbookView xWindow="7800" yWindow="2180" windowWidth="17540" windowHeight="14500" xr2:uid="{B5A9D9C6-0E32-834A-AB46-51FBAA8D7782}"/>
   </bookViews>
   <sheets>
     <sheet name="Pobreza" sheetId="2" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Pobreza!$A$1:$C$1</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,63 +36,114 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>id</t>
   </si>
   <si>
-    <t>Región</t>
-  </si>
-  <si>
-    <t>Arica y Parinacota</t>
-  </si>
-  <si>
-    <t>Tarapacá</t>
-  </si>
-  <si>
-    <t>Antofagasta</t>
-  </si>
-  <si>
-    <t>Atacama</t>
-  </si>
-  <si>
-    <t>Coquimbo</t>
-  </si>
-  <si>
-    <t>Valparaíso</t>
-  </si>
-  <si>
-    <t>Metropolitana</t>
-  </si>
-  <si>
-    <t>O’Higgins</t>
-  </si>
-  <si>
-    <t>Maule</t>
-  </si>
-  <si>
-    <t>Ñuble</t>
-  </si>
-  <si>
-    <t>Biobío</t>
-  </si>
-  <si>
-    <t>Araucanía</t>
-  </si>
-  <si>
-    <t>Los Ríos</t>
-  </si>
-  <si>
-    <t>Los Lagos</t>
-  </si>
-  <si>
-    <t>Aysén</t>
-  </si>
-  <si>
-    <t>Magallanes</t>
-  </si>
-  <si>
     <t>Pobreza</t>
+  </si>
+  <si>
+    <t>Departamento</t>
+  </si>
+  <si>
+    <t>Antioquia</t>
+  </si>
+  <si>
+    <t>Córdoba</t>
+  </si>
+  <si>
+    <t>Chocó</t>
+  </si>
+  <si>
+    <t>Sucre</t>
+  </si>
+  <si>
+    <t>Atlántico</t>
+  </si>
+  <si>
+    <t>Bolívar</t>
+  </si>
+  <si>
+    <t>Magdalena</t>
+  </si>
+  <si>
+    <t>Cesar</t>
+  </si>
+  <si>
+    <t>La Guajira</t>
+  </si>
+  <si>
+    <t>Cauca</t>
+  </si>
+  <si>
+    <t>Valle del Cauca</t>
+  </si>
+  <si>
+    <t>Huila</t>
+  </si>
+  <si>
+    <t>Caqueta</t>
+  </si>
+  <si>
+    <t>Meta</t>
+  </si>
+  <si>
+    <t>Boyacá</t>
+  </si>
+  <si>
+    <t>Cundinamarca</t>
+  </si>
+  <si>
+    <t>Caldas</t>
+  </si>
+  <si>
+    <t>Quindío</t>
+  </si>
+  <si>
+    <t>Risaralda</t>
+  </si>
+  <si>
+    <t>Tolima</t>
+  </si>
+  <si>
+    <t>Nariño</t>
+  </si>
+  <si>
+    <t>Norte de Santander</t>
+  </si>
+  <si>
+    <t>Santander</t>
+  </si>
+  <si>
+    <t>Casanare</t>
+  </si>
+  <si>
+    <t>Vaupés</t>
+  </si>
+  <si>
+    <t>Putumayo</t>
+  </si>
+  <si>
+    <t>Guainía</t>
+  </si>
+  <si>
+    <t>Vichada</t>
+  </si>
+  <si>
+    <t>Amazonas</t>
+  </si>
+  <si>
+    <t>Guaviare</t>
+  </si>
+  <si>
+    <t>Arauca</t>
+  </si>
+  <si>
+    <t>San Andrés y Providencia</t>
+  </si>
+  <si>
+    <t>Bogotá D.C.</t>
   </si>
 </sst>
 </file>
@@ -133,7 +187,9 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,15 +504,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97A5D213-D954-634A-B0A4-F81D01BA8F3C}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="31.33203125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -464,189 +522,354 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1">
-        <v>11.9</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="1">
-        <v>14</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1">
-        <v>9.3000000000000007</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1">
-        <v>9.5</v>
+        <v>40.200000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="C6" s="1">
-        <v>11.7</v>
+        <v>40.1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1">
-        <v>11.3</v>
+        <v>52.7</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1">
-        <v>9</v>
+        <v>39.799999999999997</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1">
-        <v>10</v>
+        <v>30.7</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C10" s="1">
-        <v>12.3</v>
+        <v>43.9</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="1">
-        <v>14.7</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="1">
-        <v>13.2</v>
+        <v>55.6</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C13" s="1">
-        <v>17.399999999999999</v>
+        <v>58.3</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C14" s="1">
-        <v>12.2</v>
+        <v>64.599999999999994</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="C15" s="1">
-        <v>11.3</v>
+        <v>59.4</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C16" s="1">
-        <v>6.6</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
+        <v>26</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>29</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>11</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="1">
+        <v>55.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>8</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="1">
+        <v>66.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>6</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="1">
+        <v>59.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>13</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>20</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="1">
+        <v>49.9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>21</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="1">
+        <v>56.3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>25</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>17</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="1">
+        <v>38.299999999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>18</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="1">
+        <v>35.799999999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>22</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="1">
+        <v>38.799999999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
         <v>3</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="1">
-        <v>5.7</v>
+      <c r="B29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="1">
+        <v>51.4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>19</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="1">
+        <v>45.7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>10</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="1">
+        <v>34.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>24</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>27</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>30</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C1" xr:uid="{E6563FFA-7B94-6D48-A293-BC32CCA20702}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C35">
+      <sortCondition ref="B1:B35"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>